<commit_message>
Update :: Add script parsing and showing scenario window
</commit_message>
<xml_diff>
--- a/Assets/script_data.xlsx
+++ b/Assets/script_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dntjr\Project\knou_game\Ara\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19044662-3D20-4D75-B804-C0D12AF2473D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943CD537-58C4-4C4A-9208-1EC3A103F6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="0" windowWidth="13480" windowHeight="13770" xr2:uid="{083029D4-FAA1-4227-B09F-1A7F6266207C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{083029D4-FAA1-4227-B09F-1A7F6266207C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>Monologue</t>
   </si>
@@ -335,15 +335,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,9 +347,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -370,6 +358,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCC1B45-14D5-4914-B718-5E5E1D96D16E}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,16 +721,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -738,40 +738,40 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="18">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="20"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -782,30 +782,32 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -816,16 +818,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -839,8 +841,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -854,8 +856,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -869,10 +871,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
+      <c r="A13" s="20">
         <v>2</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -881,16 +883,16 @@
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -904,8 +906,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -916,26 +918,28 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -949,8 +953,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="22"/>
+      <c r="B20" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -964,10 +968,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="11">
+      <c r="A21" s="20">
         <v>3</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -976,7 +980,7 @@
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
@@ -984,7 +988,7 @@
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="10" t="s">
         <v>20</v>
       </c>
@@ -996,17 +1000,19 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="9" t="s">
         <v>22</v>
       </c>
@@ -1014,7 +1020,7 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="9" t="s">
         <v>28</v>
       </c>
@@ -1029,7 +1035,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -1037,7 +1043,7 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="9" t="s">
         <v>20</v>
       </c>
@@ -1049,7 +1055,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="9" t="s">
         <v>20</v>
       </c>
@@ -1061,7 +1067,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="9" t="s">
         <v>20</v>
       </c>
@@ -1073,7 +1079,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="9" t="s">
         <v>22</v>
       </c>
@@ -1081,7 +1087,7 @@
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Update :: Background effect update
</commit_message>
<xml_diff>
--- a/Assets/script_data.xlsx
+++ b/Assets/script_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dntjr\Project\knou_game\Ara\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943CD537-58C4-4C4A-9208-1EC3A103F6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A93C4F-EA4A-48F1-9222-0D713815E5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{083029D4-FAA1-4227-B09F-1A7F6266207C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>Monologue</t>
   </si>
@@ -708,7 +708,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,19 +1081,19 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="21"/>
       <c r="B31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="21"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>14</v>
+      <c r="B32" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update -- Logic & scene update
- Update script data
- Add quest sequence, quest data
</commit_message>
<xml_diff>
--- a/Assets/script_data.xlsx
+++ b/Assets/script_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dntjr\Project\knou_game\Ara\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A93C4F-EA4A-48F1-9222-0D713815E5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4B6127-60D7-4300-8244-430880C266E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{083029D4-FAA1-4227-B09F-1A7F6266207C}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>옷 입기</t>
   </si>
   <si>
-    <t>옷장 앞으로 가 옷을 갈아입으세요.</t>
-  </si>
-  <si>
     <t>출근</t>
   </si>
   <si>
@@ -131,18 +128,12 @@
     <t>work clothes</t>
   </si>
   <si>
-    <t>시끄러운 알람 소리와 함께 자그마한 섬광이 비친다. 아라의 핸드폰이 울린다.</t>
-  </si>
-  <si>
     <t>BACKGROUND</t>
   </si>
   <si>
     <t>Light</t>
   </si>
   <si>
-    <t>핸드폰을 집어 든 뒤 끈다.</t>
-  </si>
-  <si>
     <t>Yejin</t>
   </si>
   <si>
@@ -164,10 +155,19 @@
     <t>recorded</t>
   </si>
   <si>
-    <t>change_clothes</t>
-  </si>
-  <si>
-    <t>go_company</t>
+    <t>(핸드폰을 집어 든 뒤 끈다.)</t>
+  </si>
+  <si>
+    <t>(시끄러운 알람 소리와 함께 자그마한 섬광이 비친다. 아라의 핸드폰이 울린다.)</t>
+  </si>
+  <si>
+    <t>거울 앞으로 가 옷을 갈아입으세요.</t>
+  </si>
+  <si>
+    <t>ChangeClothes</t>
+  </si>
+  <si>
+    <t>GoOutsideFromHome</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -221,19 +221,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -301,11 +288,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,31 +338,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -359,16 +377,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -708,7 +729,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,11 +755,11 @@
         <v>16</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -750,7 +771,7 @@
       <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="15" t="s">
         <v>21</v>
       </c>
@@ -758,31 +779,31 @@
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
-      <c r="B4" s="15" t="s">
-        <v>32</v>
+      <c r="A4" s="22"/>
+      <c r="B4" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="17">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="22"/>
+      <c r="B5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
-      <c r="B5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="18" t="s">
         <v>20</v>
       </c>
@@ -790,23 +811,23 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="12">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="18" t="s">
         <v>20</v>
       </c>
@@ -818,7 +839,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
@@ -826,7 +847,7 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="15" t="s">
         <v>23</v>
       </c>
@@ -834,46 +855,44 @@
         <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="20">
-        <v>2</v>
-      </c>
+      <c r="A13" s="23"/>
       <c r="B13" s="15" t="s">
         <v>19</v>
       </c>
@@ -883,7 +902,9 @@
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
+      <c r="A14" s="21">
+        <v>2</v>
+      </c>
       <c r="B14" s="15" t="s">
         <v>21</v>
       </c>
@@ -891,22 +912,22 @@
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
@@ -918,7 +939,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
@@ -930,7 +951,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="15" t="s">
         <v>22</v>
       </c>
@@ -938,39 +959,37 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="20">
-        <v>3</v>
-      </c>
+      <c r="A21" s="23"/>
       <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
@@ -980,7 +999,9 @@
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
+      <c r="A22" s="19">
+        <v>3</v>
+      </c>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
@@ -988,7 +1009,7 @@
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="21"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="10" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1021,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
@@ -1012,7 +1033,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="21"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="9" t="s">
         <v>22</v>
       </c>
@@ -1020,22 +1041,22 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="21"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="21"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -1043,7 +1064,7 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="21"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="9" t="s">
         <v>20</v>
       </c>
@@ -1055,7 +1076,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="9" t="s">
         <v>20</v>
       </c>
@@ -1067,7 +1088,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="21"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="9" t="s">
         <v>20</v>
       </c>
@@ -1079,7 +1100,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="21"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="9" t="s">
         <v>20</v>
       </c>
@@ -1091,7 +1112,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="9" t="s">
         <v>22</v>
       </c>
@@ -1101,9 +1122,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="A21:A32"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A22:A32"/>
+    <mergeCell ref="A14:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>